<commit_message>
files from canada june 22
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/HOIpTP/Health Outcome Incidence per Ton Pollutant.xlsx
+++ b/InputData/add-outputs/HOIpTP/Health Outcome Incidence per Ton Pollutant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\HOIpTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{DFC156A8-FA75-4A47-ABD5-FD9A05AE12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E618284-F55B-4BCD-AC7B-EE6D89491A1D}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{DFC156A8-FA75-4A47-ABD5-FD9A05AE12CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3998DBE6-2E16-4441-8986-26D09C0DF721}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="210" windowWidth="24765" windowHeight="16080" firstSheet="2" xr2:uid="{86292C8D-3CA1-4858-AA87-6B74F5B88277}"/>
+    <workbookView xWindow="2490" yWindow="210" windowWidth="24765" windowHeight="16080" activeTab="4" xr2:uid="{86292C8D-3CA1-4858-AA87-6B74F5B88277}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
     <t>Canada PM2.5 premature deaths 2016</t>
   </si>
   <si>
-    <t xml:space="preserve">deatsh per tonne </t>
+    <t xml:space="preserve">deaths per tonne </t>
   </si>
   <si>
     <t>Key to Table Numbers</t>
@@ -974,7 +974,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1066,6 +1066,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1384,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21A12EE-0370-46D8-B25C-90C403A4CDFD}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5387,7 +5388,9 @@
   </sheetPr>
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6092,8 +6095,8 @@
         <f t="array" aca="1" ref="B6" ca="1">INDIRECT(CONCATENATE("'",HLOOKUP(B$1,$B$21:$E$23,3,FALSE),"'!",$B$25,ROW($A6)+5))*About!$A$27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C6" t="e">
-        <f t="shared" ca="1" si="3"/>
+      <c r="C6" s="43" t="e">
+        <f ca="1">$B6+($F6-$B6)*(C$1-$B$1)/($F$1-$B$1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D6" t="e">
@@ -16953,7 +16956,7 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -19910,7 +19913,9 @@
   </sheetPr>
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -24294,7 +24299,7 @@
   <dimension ref="A1:AJ25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28678,7 +28683,7 @@
   </sheetPr>
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -47031,6 +47036,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
@@ -47043,13 +47057,16 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </l787e5950a9249679d0130235a9a791b>
     <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6681120aa8fa62dd7a0beb503524cb55">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b98e8ac0331400a99b3dbea3ee620024" ns2:_="" ns3:_="" ns4:_="">
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
     <xsd:import namespace="de340059-046a-4f1a-8b62-ade039df3700"/>
     <xsd:import namespace="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
@@ -47073,6 +47090,8 @@
                 <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -47159,6 +47178,18 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="26" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a296b89e-8abc-49db-b68e-edd9bb7809e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="27" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -47293,23 +47324,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF1F1E3D-E4DE-4476-A614-AA3AB65BEB47}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C58E571F-AB10-406F-B00C-FF8E75968080}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC88D51-A406-4757-BFF1-69F778ADAC30}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF1F1E3D-E4DE-4476-A614-AA3AB65BEB47}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02D8FE89-D4E9-400D-B13D-7E28A832BA8F}"/>
 </file>
</xml_diff>